<commit_message>
Added bulk rename tool
Added PyQt5 example to TextBoxCompare.py
</commit_message>
<xml_diff>
--- a/final.xlsx
+++ b/final.xlsx
@@ -496,11 +496,6 @@
           <t>Nipples 44,56</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Carbon Steel - Branch Outlets Std Weight - ButtWld</t>
-        </is>
-      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>ABOVE GROUND</t>
@@ -523,16 +518,6 @@
           <t>Fittings 57,551</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Carbon Steel - Butt Weld, Std Wt - ButtWld</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2-1/2" TO 4"</t>
-        </is>
-      </c>
       <c r="E4" t="inlineStr">
         <is>
           <t>ABOVE GROUND</t>
@@ -545,11 +530,6 @@
       </c>
     </row>
     <row r="5">
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Carbon Steel - Butt Weld, Std Wt - ButtWld Totals:</t>
-        </is>
-      </c>
       <c r="F5" t="inlineStr">
         <is>
           <t>Copper - Pressure - 95/5 Totals:</t>
@@ -557,11 +537,6 @@
       </c>
     </row>
     <row r="6">
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Copper - Pressure - 95/5 Totals:</t>
-        </is>
-      </c>
       <c r="F6" t="inlineStr">
         <is>
           <t>Copper - Propress - PP</t>
@@ -569,16 +544,6 @@
       </c>
     </row>
     <row r="7">
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Copper - Propress - PP</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>1/2" TO 2"</t>
-        </is>
-      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>Material Multiplier: F2300 - Copper ProPress -  0.55</t>
@@ -586,28 +551,13 @@
       </c>
     </row>
     <row r="8">
-      <c r="C8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>Copper - Propress - PP Totals:</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>117</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Copper - Propress - PP Totals:</t>
-        </is>
-      </c>
     </row>
     <row r="9">
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Carbon Steel - Raised Face, 150 W</t>
-        </is>
-      </c>
       <c r="F9" t="inlineStr">
         <is>
           <t>Bronze - Flanged Circuit</t>
@@ -615,11 +565,6 @@
       </c>
     </row>
     <row r="10">
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Carbon Steel - Raised Face, 150 Weldbend - Flanged</t>
-        </is>
-      </c>
       <c r="F10" t="inlineStr">
         <is>
           <t>Bronze - Flanged Circuit Setter - Flanged Totals:</t>
@@ -627,16 +572,6 @@
       </c>
     </row>
     <row r="11">
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Carbon Steel - Raised Face, 150 Weldbend - Flanged Totals:</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>2-1/2" TO 3"</t>
-        </is>
-      </c>
       <c r="F11" t="inlineStr">
         <is>
           <t>Bronze - Soldered Ball WOG - 95/5</t>
@@ -644,16 +579,6 @@
       </c>
     </row>
     <row r="12">
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Cast Iron - Flanged Y-Strainer - Flanged</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>2-1/2" TO 3"</t>
-        </is>
-      </c>
       <c r="F12" t="inlineStr">
         <is>
           <t>Material Multiplier: V0RA0 - APP - Bronze Ball Valves - APP -  0.55</t>
@@ -661,11 +586,6 @@
       </c>
     </row>
     <row r="13">
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Material Multiplier: V0NB0 - NIB - Cast Iron Gate, Globe, Check Vlvs - NIB -  0.50</t>
-        </is>
-      </c>
       <c r="F13" t="inlineStr">
         <is>
           <t>Bronze - Soldered Ball WOG - 95/5 Totals:</t>
@@ -673,16 +593,6 @@
       </c>
     </row>
     <row r="14">
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>- Copper Joints Emory Cloth -</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="F14" t="inlineStr">
         <is>
           <t>Bronze - Soldered Circuit Setter - 95/5</t>
@@ -690,16 +600,6 @@
       </c>
     </row>
     <row r="15">
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>- Copper Joints Flux -  Totals:</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="F15" t="inlineStr">
         <is>
           <t>Bronze - Soldered Circuit Setter - 95/5</t>
@@ -707,16 +607,6 @@
       </c>
     </row>
     <row r="16">
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>- Copper Joints Solder -  Totals:</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="F16" t="inlineStr">
         <is>
           <t>Bronze - Soldered Circuit Setter - 95/5 Totals:</t>
@@ -724,16 +614,6 @@
       </c>
     </row>
     <row r="17">
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Carbon Steel - Pipe Cut with Cutte</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>3" TO 4"</t>
-        </is>
-      </c>
       <c r="F17" t="inlineStr">
         <is>
           <t>Bronze - Threaded 2-Way Control - Thread</t>
@@ -741,16 +621,6 @@
       </c>
     </row>
     <row r="18">
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Copper - Pipe Cut with Cutters - Cutters</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>1/2" TO 2"</t>
-        </is>
-      </c>
       <c r="F18" t="inlineStr">
         <is>
           <t>Bronze - Threaded 2-Way Control - Thread Totals:</t>
@@ -758,16 +628,6 @@
       </c>
     </row>
     <row r="19">
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Carbon Steel - Sleeve - Floor - Inst</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>2" TO 2"</t>
-        </is>
-      </c>
       <c r="F19" t="inlineStr">
         <is>
           <t>Bronze - Threaded Y-Strainer - Thread</t>
@@ -775,16 +635,6 @@
       </c>
     </row>
     <row r="20">
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Carbon Steel - Sleeve - Floor - InstPan</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>2" TO 3"</t>
-        </is>
-      </c>
       <c r="F20" t="inlineStr">
         <is>
           <t>Material Multiplier: V0SA0 - MUL - Bronze Strainers - MUL -  0.50</t>

</xml_diff>

<commit_message>
Added Fitting class to MaterialsChart.py
</commit_message>
<xml_diff>
--- a/final.xlsx
+++ b/final.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,6 +452,16 @@
           <t>Copper - PressFit - PrssFit</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Carbon Steel</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Copper</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -484,6 +494,16 @@
           <t>Material Multiplier: P2000 - Copper Tube - CER -  0.47</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Copper</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Copper</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -685,6 +705,195 @@
     </row>
     <row r="27">
       <c r="F27" t="inlineStr">
+        <is>
+          <t>- Copper Joints Solder -  Totals:</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Copper - PressFit - PrssFit</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Material Multiplier: P2000 - Copper Tube - CER -  0.47</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Copper - PressFit - PrssFit Totals:</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Copper - Pressure - 95/5</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Copper - Pressure - 95/5 Totals:</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Copper - Propress - PP</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Material Multiplier: F2300 - Copper ProPress -  0.55</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Copper - Propress - PP Totals:</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Bronze - Flanged Circuit</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Bronze - Flanged Circuit Setter - Flanged Totals:</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Bronze - Soldered Ball WOG - 95/5</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Material Multiplier: V0RA0 - APP - Bronze Ball Valves - APP -  0.55</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Bronze - Soldered Ball WOG - 95/5 Totals:</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Bronze - Soldered Circuit Setter - 95/5</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Bronze - Soldered Circuit Setter - 95/5</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Bronze - Soldered Circuit Setter - 95/5 Totals:</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Bronze - Threaded 2-Way Control - Thread</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Bronze - Threaded 2-Way Control - Thread Totals:</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Bronze - Threaded Y-Strainer - Thread</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Material Multiplier: V0SA0 - MUL - Bronze Strainers - MUL -  0.50</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Bronze - Threaded Y-Strainer - Thread Totals:</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>- Copper Joints Emory Cloth -</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>- Copper Joints Emory Cloth -  Totals:</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>- Copper Joints Flux -</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>- Copper Joints Flux -  Totals:</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>- Copper Joints Solder -</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="F54" t="inlineStr">
         <is>
           <t>- Copper Joints Solder -  Totals:</t>
         </is>

</xml_diff>